<commit_message>
update binary growth results on CGXII #5
</commit_message>
<xml_diff>
--- a/growth_binary/binary_growth_metabolites.xlsx
+++ b/growth_binary/binary_growth_metabolites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baeuerle/Organisation/Masterarbeit/C_striatum_wetlab/growth_binary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A164C81-0826-3143-8906-48D7C9A85B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7312C919-4555-C242-A182-40787C679AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="1" xr2:uid="{EA9A150F-2AE7-6A42-980C-393C02D847AE}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="35840" windowHeight="21900" activeTab="1" xr2:uid="{EA9A150F-2AE7-6A42-980C-393C02D847AE}"/>
   </bookViews>
   <sheets>
     <sheet name="CGXII" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t>BiGG</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>cobalt 1 + nicotinic acid 1 + pantothenic acid  1</t>
+  </si>
+  <si>
+    <t>OD600 (after 19h)</t>
+  </si>
+  <si>
+    <t>maybe waited too long before logphase</t>
   </si>
 </sst>
 </file>
@@ -690,10 +696,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5606AF43-B6C7-D043-8B00-297C630415FD}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -702,7 +708,7 @@
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -719,7 +725,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -736,7 +742,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -753,7 +759,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -770,7 +776,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -787,7 +793,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -828,7 +834,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -869,7 +875,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -910,15 +916,51 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="2">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.9E-2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.109</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.114</v>
+      </c>
+      <c r="F13" s="2">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="H13" s="2">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="I13" s="2">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="K13" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L13" s="2">
+        <v>2.4E-2</v>
+      </c>
+      <c r="M13" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -926,7 +968,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -934,7 +976,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>

</xml_diff>